<commit_message>
program chnged with create table also from program
</commit_message>
<xml_diff>
--- a/Students.xlsx
+++ b/Students.xlsx
@@ -16,18 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Rajesh</t>
   </si>
   <si>
-    <t>Student Name</t>
-  </si>
-  <si>
     <t>Progress</t>
   </si>
   <si>
     <t>Marks</t>
+  </si>
+  <si>
+    <t>Student_Name</t>
+  </si>
+  <si>
+    <t>veera</t>
+  </si>
+  <si>
+    <t>rank</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -372,18 +378,21 @@
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="D1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -392,6 +401,23 @@
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>